<commit_message>
Also update excel workbook.
</commit_message>
<xml_diff>
--- a/velfg/results_velfg_excel.xlsx
+++ b/velfg/results_velfg_excel.xlsx
@@ -1,22 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\rob\git\sycl-kernels-mem-reduced\velfg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{A07607E9-0DEF-490A-83CA-B0CC2E9383F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{965BA528-54C1-419F-A83B-1404822276E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="results_velfg" sheetId="1" r:id="rId1"/>
     <sheet name="Num CUs" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -140,7 +152,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -950,25 +962,25 @@
             <c:numRef>
               <c:f>results_velfg!$B$21:$G$21</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>10303.8490600599</c:v>
+                  <c:v>154840.57442412199</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6379.2122736044103</c:v>
+                  <c:v>146021.521949874</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6578.5199142355896</c:v>
+                  <c:v>158809.828171687</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7055.9796160588803</c:v>
+                  <c:v>144640.274280816</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5993.1929166872196</c:v>
+                  <c:v>159694.71802600601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6232.9619902505601</c:v>
+                  <c:v>158850.448829523</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2220,7 +2232,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$21</c15:sqref>
@@ -2261,7 +2273,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$18:$G$18</c15:sqref>
@@ -2293,7 +2305,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$21:$G$21</c15:sqref>
@@ -2301,31 +2313,31 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>#,##0.00</c:formatCode>
+                      <c:formatCode>General</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>10303.8490600599</c:v>
+                        <c:v>154840.57442412199</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>6379.2122736044103</c:v>
+                        <c:v>146021.521949874</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>6578.5199142355896</c:v>
+                        <c:v>158809.828171687</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>7055.9796160588803</c:v>
+                        <c:v>144640.274280816</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>5993.1929166872196</c:v>
+                        <c:v>159694.71802600601</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>6232.9619902505601</c:v>
+                        <c:v>158850.448829523</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-3411-491A-B7AE-E20E7E9D397B}"/>
                   </c:ext>
@@ -2338,7 +2350,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$22</c15:sqref>
@@ -2379,7 +2391,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$18:$G$18</c15:sqref>
@@ -2411,7 +2423,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$22:$G$22</c15:sqref>
@@ -2443,7 +2455,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-3411-491A-B7AE-E20E7E9D397B}"/>
                   </c:ext>
@@ -2456,7 +2468,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$23</c15:sqref>
@@ -2497,7 +2509,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$18:$G$18</c15:sqref>
@@ -2529,7 +2541,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$23:$G$23</c15:sqref>
@@ -2561,7 +2573,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-3411-491A-B7AE-E20E7E9D397B}"/>
                   </c:ext>
@@ -2574,7 +2586,7 @@
                 <c:order val="10"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$30</c15:sqref>
@@ -2621,7 +2633,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$18:$G$18</c15:sqref>
@@ -2653,7 +2665,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$30:$G$30</c15:sqref>
@@ -2685,7 +2697,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000A-3411-491A-B7AE-E20E7E9D397B}"/>
                   </c:ext>
@@ -2698,7 +2710,7 @@
                 <c:order val="11"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$31</c15:sqref>
@@ -2745,7 +2757,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$18:$G$18</c15:sqref>
@@ -2777,7 +2789,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$31:$G$31</c15:sqref>
@@ -2809,7 +2821,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000000B-3411-491A-B7AE-E20E7E9D397B}"/>
                   </c:ext>
@@ -3483,7 +3495,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$21</c15:sqref>
@@ -3562,7 +3574,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$21:$G$21</c15:sqref>
@@ -3570,31 +3582,31 @@
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
-                      <c:formatCode>#,##0.00</c:formatCode>
+                      <c:formatCode>General</c:formatCode>
                       <c:ptCount val="6"/>
                       <c:pt idx="0">
-                        <c:v>10303.8490600599</c:v>
+                        <c:v>154840.57442412199</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>6379.2122736044103</c:v>
+                        <c:v>146021.521949874</c:v>
                       </c:pt>
                       <c:pt idx="2">
-                        <c:v>6578.5199142355896</c:v>
+                        <c:v>158809.828171687</c:v>
                       </c:pt>
                       <c:pt idx="3">
-                        <c:v>7055.9796160588803</c:v>
+                        <c:v>144640.274280816</c:v>
                       </c:pt>
                       <c:pt idx="4">
-                        <c:v>5993.1929166872196</c:v>
+                        <c:v>159694.71802600601</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>6232.9619902505601</c:v>
+                        <c:v>158850.448829523</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-FF16-4892-9D87-6FE0AEE03AA6}"/>
                   </c:ext>
@@ -3607,7 +3619,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$22</c15:sqref>
@@ -3686,7 +3698,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$22:$G$22</c15:sqref>
@@ -3718,7 +3730,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-FF16-4892-9D87-6FE0AEE03AA6}"/>
                   </c:ext>
@@ -3731,7 +3743,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$23</c15:sqref>
@@ -3810,7 +3822,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$23:$G$23</c15:sqref>
@@ -3842,7 +3854,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-FF16-4892-9D87-6FE0AEE03AA6}"/>
                   </c:ext>
@@ -3855,7 +3867,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$24</c15:sqref>
@@ -3934,7 +3946,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$24:$G$24</c15:sqref>
@@ -3966,7 +3978,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000004-FF16-4892-9D87-6FE0AEE03AA6}"/>
                   </c:ext>
@@ -3979,7 +3991,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$25</c15:sqref>
@@ -4058,7 +4070,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$25:$G$25</c15:sqref>
@@ -4090,7 +4102,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-FF16-4892-9D87-6FE0AEE03AA6}"/>
                   </c:ext>
@@ -4103,7 +4115,7 @@
                 <c:order val="6"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$26</c15:sqref>
@@ -4188,7 +4200,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$26:$G$26</c15:sqref>
@@ -4220,7 +4232,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000006-FF16-4892-9D87-6FE0AEE03AA6}"/>
                   </c:ext>
@@ -4233,7 +4245,7 @@
                 <c:order val="7"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$27</c15:sqref>
@@ -4318,7 +4330,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$27:$G$27</c15:sqref>
@@ -4350,7 +4362,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000007-FF16-4892-9D87-6FE0AEE03AA6}"/>
                   </c:ext>
@@ -4363,7 +4375,7 @@
                 <c:order val="8"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$28</c15:sqref>
@@ -4448,7 +4460,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$28:$G$28</c15:sqref>
@@ -4480,7 +4492,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000008-FF16-4892-9D87-6FE0AEE03AA6}"/>
                   </c:ext>
@@ -4493,7 +4505,7 @@
                 <c:order val="9"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$A$29</c15:sqref>
@@ -4578,7 +4590,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>results_velfg!$B$29:$G$29</c15:sqref>
@@ -4610,7 +4622,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-FF16-4892-9D87-6FE0AEE03AA6}"/>
                   </c:ext>
@@ -7847,23 +7859,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.3828125" style="1" customWidth="1"/>
-    <col min="2" max="7" width="9.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.23046875" style="1"/>
-    <col min="9" max="9" width="22.3828125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.23046875" style="1"/>
+    <col min="1" max="1" width="20.33203125" style="1" customWidth="1"/>
+    <col min="2" max="7" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" style="1"/>
+    <col min="9" max="9" width="22.33203125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.21875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7871,7 +7883,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -7912,7 +7924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -7939,26 +7951,26 @@
       </c>
       <c r="J3" s="1">
         <f>B4/B5</f>
-        <v>0.36684335859684469</v>
+        <v>5.5127201531889414</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" ref="K3:O3" si="0">C4/C5</f>
-        <v>0.2271283089948665</v>
+        <f>C4/C5</f>
+        <v>5.1990151659575154</v>
       </c>
       <c r="L3" s="1">
-        <f t="shared" si="0"/>
-        <v>0.24682525501916705</v>
+        <f>D4/D5</f>
+        <v>5.9585251468500759</v>
       </c>
       <c r="M3" s="1">
-        <f t="shared" si="0"/>
-        <v>0.28103923255332813</v>
+        <f>E4/E5</f>
+        <v>5.7610131961929252</v>
       </c>
       <c r="N3" s="1">
-        <f t="shared" si="0"/>
-        <v>0.23083247011624661</v>
+        <f>F4/F5</f>
+        <v>6.1507658336546216</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -7988,46 +8000,46 @@
         <v>10.330387931454592</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:O4" si="1">C6/C7</f>
+        <f>C6/C7</f>
         <v>9.8413502630210861</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" si="1"/>
+        <f>D6/D7</f>
         <v>8.3451306674365693</v>
       </c>
       <c r="M4" s="1">
-        <f t="shared" si="1"/>
+        <f>E6/E7</f>
         <v>8.8212129582133123</v>
       </c>
       <c r="N4" s="1">
-        <f t="shared" si="1"/>
+        <f>F6/F7</f>
         <v>8.6681605047403512</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2">
-        <v>87.346000000000004</v>
-      </c>
-      <c r="C5" s="2">
-        <v>564.33299999999997</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1231.28</v>
-      </c>
-      <c r="E5" s="2">
-        <v>4591.8500000000004</v>
-      </c>
-      <c r="F5" s="2">
-        <v>12163.8</v>
-      </c>
-      <c r="G5" s="2">
-        <v>52126.1</v>
+      <c r="B5">
+        <v>5.81243</v>
+      </c>
+      <c r="C5">
+        <v>24.6539</v>
+      </c>
+      <c r="D5">
+        <v>51.004399999999997</v>
+      </c>
+      <c r="E5">
+        <v>224.00399999999999</v>
+      </c>
+      <c r="F5">
+        <v>456.49599999999998</v>
+      </c>
+      <c r="G5">
+        <v>2045.32</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -8053,7 +8065,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -8094,7 +8106,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>19</v>
       </c>
@@ -8117,31 +8129,31 @@
         <v>46643.788</v>
       </c>
       <c r="J8" s="1">
-        <f>B8/B7</f>
+        <f t="shared" ref="J8:O8" si="0">B8/B7</f>
         <v>25.694586581365023</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" ref="K8:O8" si="2">C8/C7</f>
+        <f t="shared" si="0"/>
         <v>22.606331891196504</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>18.898853512379411</v>
       </c>
       <c r="M8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>18.64531823383183</v>
       </c>
       <c r="N8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>19.507437108358079</v>
       </c>
       <c r="O8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>18.020664902350919</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -8164,7 +8176,7 @@
         <v>3591.3049999999998</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
@@ -8187,7 +8199,7 @@
         <v>47976.6</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>22</v>
       </c>
@@ -8210,7 +8222,7 @@
         <v>19995.2</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>23</v>
       </c>
@@ -8233,7 +8245,7 @@
         <v>3577.73</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -8256,7 +8268,7 @@
         <v>819.12</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>25</v>
       </c>
@@ -8279,7 +8291,7 @@
         <v>3623.72</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>26</v>
       </c>
@@ -8302,12 +8314,12 @@
         <v>1484.72</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
@@ -8330,7 +8342,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -8353,7 +8365,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
@@ -8376,30 +8388,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A21" s="1" t="s">
+    <row r="21" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>11</v>
       </c>
-      <c r="B21" s="1">
-        <v>10303.8490600599</v>
-      </c>
-      <c r="C21" s="1">
-        <v>6379.2122736044103</v>
-      </c>
-      <c r="D21" s="1">
-        <v>6578.5199142355896</v>
-      </c>
-      <c r="E21" s="1">
-        <v>7055.9796160588803</v>
-      </c>
-      <c r="F21" s="1">
-        <v>5993.1929166872196</v>
-      </c>
-      <c r="G21" s="1">
-        <v>6232.9619902505601</v>
+      <c r="B21">
+        <v>154840.57442412199</v>
+      </c>
+      <c r="C21">
+        <v>146021.521949874</v>
+      </c>
+      <c r="D21">
+        <v>158809.828171687</v>
+      </c>
+      <c r="E21">
+        <v>144640.274280816</v>
+      </c>
+      <c r="F21">
+        <v>159694.71802600601</v>
+      </c>
+      <c r="G21">
+        <v>158850.448829523</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>12</v>
       </c>
@@ -8422,7 +8434,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>13</v>
       </c>
@@ -8445,7 +8457,7 @@
         <v>125523.982459868</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -8468,7 +8480,7 @@
         <v>6965.55777159436</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>20</v>
       </c>
@@ -8491,7 +8503,7 @@
         <v>90468.506573515697</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>21</v>
       </c>
@@ -8514,7 +8526,7 @@
         <v>6772.0513750453301</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>22</v>
       </c>
@@ -8537,7 +8549,7 @@
         <v>16248.8997359366</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -8560,7 +8572,7 @@
         <v>90811.771709994806</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>24</v>
       </c>
@@ -8583,7 +8595,7 @@
         <v>341024.75894392398</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>25</v>
       </c>
@@ -8606,7 +8618,7 @@
         <v>89659.245195544907</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>26</v>
       </c>
@@ -8629,12 +8641,12 @@
         <v>218829.13950105</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -8657,7 +8669,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>8</v>
       </c>
@@ -8680,7 +8692,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>10</v>
       </c>
@@ -8703,30 +8715,30 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A37" s="1" t="s">
+    <row r="37" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>11</v>
       </c>
-      <c r="B37" s="1">
-        <v>340</v>
-      </c>
-      <c r="C37" s="1">
-        <v>340</v>
-      </c>
-      <c r="D37" s="1">
-        <v>340</v>
-      </c>
-      <c r="E37" s="1">
-        <v>340</v>
-      </c>
-      <c r="F37" s="1">
-        <v>340</v>
-      </c>
-      <c r="G37" s="1">
-        <v>340</v>
+      <c r="B37">
+        <v>350</v>
+      </c>
+      <c r="C37">
+        <v>350</v>
+      </c>
+      <c r="D37">
+        <v>350</v>
+      </c>
+      <c r="E37">
+        <v>350</v>
+      </c>
+      <c r="F37">
+        <v>350</v>
+      </c>
+      <c r="G37">
+        <v>350</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>12</v>
       </c>
@@ -8749,7 +8761,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>13</v>
       </c>
@@ -8772,12 +8784,12 @@
         <v>467</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>1</v>
       </c>
@@ -8800,7 +8812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>8</v>
       </c>
@@ -8823,7 +8835,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>10</v>
       </c>
@@ -8846,30 +8858,30 @@
         <v>215</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A45" s="1" t="s">
+    <row r="45" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>11</v>
       </c>
-      <c r="B45" s="1">
-        <v>242</v>
-      </c>
-      <c r="C45" s="1">
-        <v>243</v>
-      </c>
-      <c r="D45" s="1">
-        <v>235</v>
-      </c>
-      <c r="E45" s="1">
-        <v>254</v>
-      </c>
-      <c r="F45" s="1">
-        <v>228</v>
-      </c>
-      <c r="G45" s="1">
-        <v>230</v>
+      <c r="B45">
+        <v>250</v>
+      </c>
+      <c r="C45">
+        <v>236</v>
+      </c>
+      <c r="D45">
+        <v>253</v>
+      </c>
+      <c r="E45">
+        <v>236</v>
+      </c>
+      <c r="F45">
+        <v>250</v>
+      </c>
+      <c r="G45">
+        <v>253</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>12</v>
       </c>
@@ -8892,7 +8904,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>13</v>
       </c>
@@ -8915,12 +8927,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>1</v>
       </c>
@@ -8943,7 +8955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>8</v>
       </c>
@@ -8966,7 +8978,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>10</v>
       </c>
@@ -8989,30 +9001,30 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A53" s="1" t="s">
+    <row r="53" spans="1:7" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>11</v>
       </c>
-      <c r="B53" s="1">
-        <v>156.70099999999999</v>
-      </c>
-      <c r="C53" s="1">
-        <v>665.56600000000003</v>
-      </c>
-      <c r="D53" s="1">
-        <v>1393.71</v>
-      </c>
-      <c r="E53" s="1">
-        <v>5097.59</v>
-      </c>
-      <c r="F53" s="1">
-        <v>13173.7</v>
-      </c>
-      <c r="G53" s="1">
-        <v>56487.6</v>
+      <c r="B53">
+        <v>64.672700000000006</v>
+      </c>
+      <c r="C53">
+        <v>108.114</v>
+      </c>
+      <c r="D53">
+        <v>174.97200000000001</v>
+      </c>
+      <c r="E53">
+        <v>583.58199999999999</v>
+      </c>
+      <c r="F53">
+        <v>1212.8699999999999</v>
+      </c>
+      <c r="G53">
+        <v>5409.18</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>12</v>
       </c>
@@ -9035,7 +9047,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>13</v>
       </c>
@@ -9058,17 +9070,17 @@
         <v>5864.28</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>33</v>
       </c>
@@ -9081,24 +9093,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.61328125" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -9121,7 +9133,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -9144,7 +9156,7 @@
         <v>2588.35</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -9167,7 +9179,7 @@
         <v>6423.07</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -9190,7 +9202,7 @@
         <v>4046.34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -9213,7 +9225,7 @@
         <v>3719.83</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>17</v>
       </c>
@@ -9236,7 +9248,7 @@
         <v>3383.21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -9259,12 +9271,12 @@
         <v>5024.1400000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -9287,7 +9299,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -9310,7 +9322,7 @@
         <v>125523.982459868</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -9333,7 +9345,7 @@
         <v>50583.288053843396</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -9356,7 +9368,7 @@
         <v>80294.784916739503</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -9379,7 +9391,7 @@
         <v>87342.701144944804</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -9402,7 +9414,7 @@
         <v>96033.057362682099</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -9425,12 +9437,12 @@
         <v>64667.783939141802</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>1</v>
       </c>
@@ -9453,7 +9465,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -9476,7 +9488,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>14</v>
       </c>
@@ -9499,7 +9511,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>15</v>
       </c>
@@ -9522,7 +9534,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
@@ -9545,7 +9557,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>17</v>
       </c>
@@ -9568,7 +9580,7 @@
         <v>1261</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>18</v>
       </c>
@@ -9591,12 +9603,12 @@
         <v>1707</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -9619,7 +9631,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -9642,7 +9654,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -9665,7 +9677,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>15</v>
       </c>
@@ -9688,7 +9700,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>16</v>
       </c>
@@ -9711,7 +9723,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>17</v>
       </c>
@@ -9734,7 +9746,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>18</v>
       </c>
@@ -9757,17 +9769,17 @@
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>1</v>
       </c>
@@ -9775,7 +9787,7 @@
         <v>125523.982459868</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2</v>
       </c>
@@ -9783,7 +9795,7 @@
         <v>50583.288053843396</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>3</v>
       </c>
@@ -9791,7 +9803,7 @@
         <v>80294.784916739503</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>4</v>
       </c>
@@ -9799,7 +9811,7 @@
         <v>87342.701144944804</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>5</v>
       </c>
@@ -9807,7 +9819,7 @@
         <v>96033.057362682099</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>6</v>
       </c>

</xml_diff>